<commit_message>
conftest file updated for headless
</commit_message>
<xml_diff>
--- a/TestData/SignIn_Data.xlsx
+++ b/TestData/SignIn_Data.xlsx
@@ -2,40 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn_Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -49,27 +37,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -79,23 +52,17 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -467,22 +434,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Message</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Result</t>
         </is>

</xml_diff>